<commit_message>
Read External Data from Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/Book1.xlsx
+++ b/src/test/resources/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvaro.meza\Documents\eclipse-workspace\ScreenCucumberDataTable\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D8FC652F-ED10-424A-AD78-68129E26BF92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9147D4FF-0E7B-464F-8DF6-03E8CAC1C9CB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{B2318032-BA3D-465E-984A-BDCC3F0D4969}"/>
   </bookViews>
@@ -30,10 +30,10 @@
     <t>name</t>
   </si>
   <si>
-    <t>sebastian baron</t>
+    <t>Sebastian Baron Caicedo</t>
   </si>
   <si>
-    <t>luis carlos covilla</t>
+    <t>Luis Carlos Covilla Yarce</t>
   </si>
 </sst>
 </file>
@@ -69,8 +69,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +405,12 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>